<commit_message>
callback hell and presentation materials
</commit_message>
<xml_diff>
--- a/thinkful stuff.xlsx
+++ b/thinkful stuff.xlsx
@@ -450,80 +450,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A2:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
@@ -532,6 +523,15 @@
       </c>
     </row>
     <row r="7" spans="1:11">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
@@ -553,7 +553,7 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -572,31 +572,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="D20" t="s">
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="D21" t="s">
+    <row r="21" spans="1:2">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>